<commit_message>
New results added code modified
</commit_message>
<xml_diff>
--- a/Models/Results/mean_mcc_score.xlsx
+++ b/Models/Results/mean_mcc_score.xlsx
@@ -4,17 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22451" windowHeight="10464"/>
+    <workbookView windowWidth="18551" windowHeight="10464"/>
   </bookViews>
   <sheets>
     <sheet name="mean_mcc_score" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <pivotCaches>
+    <pivotCache cacheId="0" r:id="rId2"/>
+  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31">
   <si>
     <t>DT</t>
   </si>
@@ -38,6 +41,9 @@
   </si>
   <si>
     <t>ExpME</t>
+  </si>
+  <si>
+    <t>Winner</t>
   </si>
   <si>
     <t>AEEEM-EQ</t>
@@ -112,9 +118,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -126,9 +132,69 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -137,6 +203,22 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -151,82 +233,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,7 +254,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -256,7 +262,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -278,31 +284,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -314,7 +398,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -326,43 +410,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -374,101 +464,148 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="18">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFABABAB"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFABABAB"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFABABAB"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFABABAB"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFABABAB"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFABABAB"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFABABAB"/>
+      </right>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFABABAB"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFABABAB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFABABAB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFABABAB"/>
+      </right>
+      <top style="thin">
+        <color indexed="65"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFABABAB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -483,6 +620,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -511,24 +672,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -543,184 +686,185 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -782,6 +926,110 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" refreshedDate="44733.8339930556" refreshedBy="AdityaShankar" recordCount="21">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="K2:K23" sheet="mean_mcc_score"/>
+  </cacheSource>
+  <cacheFields count="1">
+    <cacheField name="LOG" numFmtId="0">
+      <sharedItems count="7">
+        <s v="LOG"/>
+        <s v="ImpME"/>
+        <s v="Bagging"/>
+        <s v="ExpME"/>
+        <s v="KNN"/>
+        <s v="SVM"/>
+        <s v="Adaboost"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="21">
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" autoFormatId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" createdVersion="5" useAutoFormatting="1" compact="0" indent="0" outline="1" compactData="0" outlineData="1" showDrill="1" multipleFieldFilters="0">
+  <location ref="B28:D45" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="1">
+    <pivotField compact="0" showAll="0"/>
+  </pivotFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1042,10 +1290,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="B29" sqref="B29:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4"/>
@@ -1053,7 +1301,7 @@
     <col min="1" max="1" width="17.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9">
+    <row r="1" spans="2:11">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1078,10 +1326,13 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>0.395125105616329</v>
@@ -1107,10 +1358,13 @@
       <c r="I2">
         <v>0.524192291593037</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>0.394130168621109</v>
@@ -1136,10 +1390,13 @@
       <c r="I3">
         <v>0.511676394356141</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>0.158111330779917</v>
@@ -1165,10 +1422,13 @@
       <c r="I4">
         <v>0.235617715148349</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="K4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>0.316887090229071</v>
@@ -1194,10 +1454,13 @@
       <c r="I5">
         <v>0.339864398788174</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="K5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>0.196079177130588</v>
@@ -1223,10 +1486,13 @@
       <c r="I6">
         <v>0.329523653855798</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="K6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>0.533172661871934</v>
@@ -1252,10 +1518,13 @@
       <c r="I7">
         <v>0.659684057857487</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="K7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>0.330373090368999</v>
@@ -1281,10 +1550,13 @@
       <c r="I8">
         <v>0.478621380738973</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="K8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>0.437432088503855</v>
@@ -1310,10 +1582,13 @@
       <c r="I9">
         <v>0.546789273087758</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="K9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>0.376326659066263</v>
@@ -1339,10 +1614,13 @@
       <c r="I10">
         <v>0.538216592177374</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="K10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>0.533160285935644</v>
@@ -1368,10 +1646,13 @@
       <c r="I11">
         <v>0.601251730008091</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="K11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12">
         <v>0.532889561010013</v>
@@ -1397,10 +1678,13 @@
       <c r="I12">
         <v>0.582598140689429</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="K12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13">
         <v>0.33289190494115</v>
@@ -1426,10 +1710,13 @@
       <c r="I13">
         <v>0.400383270753121</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="K13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14">
         <v>0.271242939909101</v>
@@ -1455,10 +1742,13 @@
       <c r="I14">
         <v>0.469175340182235</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="K14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>0.204291293936022</v>
@@ -1484,10 +1774,13 @@
       <c r="I15">
         <v>0.308791321621201</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="K15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16">
         <v>0.161560172670028</v>
@@ -1513,10 +1806,13 @@
       <c r="I16">
         <v>0.0957826320533722</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="K16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B17">
         <v>0.378478597698636</v>
@@ -1542,10 +1838,13 @@
       <c r="I17">
         <v>0.435323549368269</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="K17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18">
         <v>0.459580522432316</v>
@@ -1571,10 +1870,13 @@
       <c r="I18">
         <v>0.587876685100826</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="K18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B19">
         <v>0.236951350884257</v>
@@ -1600,10 +1902,13 @@
       <c r="I19">
         <v>0.180738759983555</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="K19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20">
         <v>0.316444814128155</v>
@@ -1629,10 +1934,13 @@
       <c r="I20">
         <v>0.458570702667934</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="K20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21">
         <v>0.27486980544159</v>
@@ -1658,10 +1966,13 @@
       <c r="I21">
         <v>0.456267433299866</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="K21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22">
         <v>0.230842044163601</v>
@@ -1687,10 +1998,13 @@
       <c r="I22">
         <v>0.313754851528434</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="K22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23">
         <v>0.370673683859545</v>
@@ -1716,6 +2030,99 @@
       <c r="I23">
         <v>0.445606773858918</v>
       </c>
+      <c r="K23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="1"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="4"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="4"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="4"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" s="4"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="6"/>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="6"/>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="B38" s="4"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="B39" s="4"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="6"/>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40" s="4"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="6"/>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="B41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" spans="2:4">
+      <c r="B42" s="4"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="6"/>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="B43" s="4"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="6"/>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="B44" s="4"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="6"/>
+    </row>
+    <row r="45" spans="2:4">
+      <c r="B45" s="7"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>